<commit_message>
Renamed utility plant folder correctly; extended POU series to 2006; added SMUD data for 2012 and 2006-10
</commit_message>
<xml_diff>
--- a/AppendixTables/Total O&M POUs-only.xlsx
+++ b/AppendixTables/Total O&M POUs-only.xlsx
@@ -1,20 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10811"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10908"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rayan/Developer/CCAResearch/ConsolidatedPrimerData/CA_electricity_primer/AppendixTables/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2B2E0C31-97F2-884E-BA8A-D9A26964DD10}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A8C2B4D9-72A2-0649-B420-F230E8963962}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="25600" windowHeight="15500" xr2:uid="{EE6E0027-42E0-E74F-9685-559680A93D52}"/>
+    <workbookView xWindow="0" yWindow="18500" windowWidth="28800" windowHeight="15820" xr2:uid="{EE6E0027-42E0-E74F-9685-559680A93D52}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$C$37</definedName>
+  </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -36,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="5">
   <si>
     <t>SMUD</t>
   </si>
@@ -57,10 +60,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="1">
-    <numFmt numFmtId="175" formatCode="\$##0"/>
-  </numFmts>
-  <fonts count="4">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -74,16 +74,6 @@
       <color theme="1"/>
       <name val="Aptos Narrow"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="9"/>
-      <color theme="1"/>
-      <name val="CIDFont+F2"/>
-    </font>
-    <font>
-      <sz val="9"/>
-      <color theme="1"/>
-      <name val="TimesNewRomanPSMT"/>
     </font>
   </fonts>
   <fills count="2">
@@ -106,12 +96,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="175" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="175" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="175" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -446,19 +433,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{09B6FE2E-2FCD-6348-B33B-60CC5A0315DF}">
-  <dimension ref="A1:D29"/>
+  <dimension ref="A1:D37"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="150" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+    <sheetView tabSelected="1" topLeftCell="A17" zoomScale="150" workbookViewId="0">
+      <selection activeCell="C28" sqref="C28"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="3" max="3" width="27.5" customWidth="1"/>
+    <col min="3" max="3" width="53" customWidth="1"/>
     <col min="4" max="4" width="34.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>4</v>
       </c>
@@ -470,313 +457,408 @@
       </c>
       <c r="D1" s="1"/>
     </row>
-    <row r="2" spans="1:4">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>1</v>
       </c>
       <c r="B2">
+        <v>2006</v>
+      </c>
+      <c r="C2">
+        <v>2286921000</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B3">
+        <v>2007</v>
+      </c>
+      <c r="C3">
+        <v>2266236000</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>1</v>
+      </c>
+      <c r="B4">
+        <v>2008</v>
+      </c>
+      <c r="C4">
+        <v>2457597000</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>1</v>
+      </c>
+      <c r="B5">
+        <v>2009</v>
+      </c>
+      <c r="C5">
+        <v>2336431000</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>1</v>
+      </c>
+      <c r="B6">
         <v>2010</v>
       </c>
-      <c r="C2" s="2">
+      <c r="C6">
         <v>2625300000</v>
       </c>
     </row>
-    <row r="3" spans="1:4">
-      <c r="A3" t="s">
-        <v>1</v>
-      </c>
-      <c r="B3">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>1</v>
+      </c>
+      <c r="B7">
         <v>2011</v>
       </c>
-      <c r="C3" s="2">
+      <c r="C7">
         <v>2695125000</v>
       </c>
     </row>
-    <row r="4" spans="1:4">
-      <c r="A4" t="s">
-        <v>1</v>
-      </c>
-      <c r="B4">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>1</v>
+      </c>
+      <c r="B8">
         <v>2012</v>
       </c>
-      <c r="C4" s="2">
+      <c r="C8">
         <v>2629541000</v>
       </c>
     </row>
-    <row r="5" spans="1:4">
-      <c r="A5" t="s">
-        <v>1</v>
-      </c>
-      <c r="B5">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>1</v>
+      </c>
+      <c r="B9">
         <v>2013</v>
       </c>
-      <c r="C5" s="2">
+      <c r="C9">
         <v>2684734000</v>
       </c>
     </row>
-    <row r="6" spans="1:4">
-      <c r="A6" t="s">
-        <v>1</v>
-      </c>
-      <c r="B6">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>1</v>
+      </c>
+      <c r="B10">
         <v>2014</v>
       </c>
-      <c r="C6" s="2">
+      <c r="C10">
         <v>2830383000</v>
       </c>
     </row>
-    <row r="7" spans="1:4">
-      <c r="A7" t="s">
-        <v>1</v>
-      </c>
-      <c r="B7">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>1</v>
+      </c>
+      <c r="B11">
         <v>2015</v>
       </c>
-      <c r="C7" s="2">
+      <c r="C11">
         <v>2941246000</v>
       </c>
     </row>
-    <row r="8" spans="1:4">
-      <c r="A8" t="s">
-        <v>1</v>
-      </c>
-      <c r="B8">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>1</v>
+      </c>
+      <c r="B12">
         <v>2016</v>
       </c>
-      <c r="C8" s="2">
+      <c r="C12">
         <v>2992412000</v>
       </c>
     </row>
-    <row r="9" spans="1:4">
-      <c r="A9" t="s">
-        <v>1</v>
-      </c>
-      <c r="B9">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
+        <v>1</v>
+      </c>
+      <c r="B13">
         <v>2017</v>
       </c>
-      <c r="C9" s="2">
+      <c r="C13">
         <v>3086198000</v>
       </c>
     </row>
-    <row r="10" spans="1:4">
-      <c r="A10" t="s">
-        <v>1</v>
-      </c>
-      <c r="B10">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
+        <v>1</v>
+      </c>
+      <c r="B14">
         <v>2018</v>
       </c>
-      <c r="C10" s="2">
+      <c r="C14">
         <v>3078962000</v>
       </c>
     </row>
-    <row r="11" spans="1:4">
-      <c r="A11" t="s">
-        <v>1</v>
-      </c>
-      <c r="B11">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
+        <v>1</v>
+      </c>
+      <c r="B15">
         <v>2019</v>
       </c>
-      <c r="C11" s="2">
+      <c r="C15">
         <v>3558620000</v>
       </c>
     </row>
-    <row r="12" spans="1:4">
-      <c r="A12" t="s">
-        <v>1</v>
-      </c>
-      <c r="B12">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
+        <v>1</v>
+      </c>
+      <c r="B16">
         <v>2020</v>
       </c>
-      <c r="C12" s="2">
+      <c r="C16">
         <v>3443310000</v>
       </c>
     </row>
-    <row r="13" spans="1:4">
-      <c r="A13" t="s">
-        <v>1</v>
-      </c>
-      <c r="B13">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A17" t="s">
+        <v>1</v>
+      </c>
+      <c r="B17">
         <v>2021</v>
       </c>
-      <c r="C13" s="2">
+      <c r="C17">
         <v>3524339000</v>
       </c>
     </row>
-    <row r="14" spans="1:4">
-      <c r="A14" t="s">
-        <v>1</v>
-      </c>
-      <c r="B14">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A18" t="s">
+        <v>1</v>
+      </c>
+      <c r="B18">
         <v>2022</v>
       </c>
-      <c r="C14" s="2">
+      <c r="C18">
         <v>3792772000</v>
       </c>
     </row>
-    <row r="15" spans="1:4">
-      <c r="A15" t="s">
-        <v>1</v>
-      </c>
-      <c r="B15">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A19" t="s">
+        <v>1</v>
+      </c>
+      <c r="B19">
         <v>2023</v>
       </c>
-      <c r="C15" s="2">
+      <c r="C19">
         <v>4216363000</v>
       </c>
     </row>
-    <row r="16" spans="1:4">
-      <c r="A16" t="s">
-        <v>0</v>
-      </c>
-      <c r="B16">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A20" t="s">
+        <v>0</v>
+      </c>
+      <c r="B20">
+        <v>2006</v>
+      </c>
+      <c r="C20">
+        <v>1165547000</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A21" t="s">
+        <v>0</v>
+      </c>
+      <c r="B21">
+        <v>2007</v>
+      </c>
+      <c r="C21">
+        <v>1216905000</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A22" t="s">
+        <v>0</v>
+      </c>
+      <c r="B22">
+        <v>2008</v>
+      </c>
+      <c r="C22">
+        <v>1486679000</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A23" t="s">
+        <v>0</v>
+      </c>
+      <c r="B23">
+        <v>2009</v>
+      </c>
+      <c r="C23">
+        <v>1293337000</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A24" t="s">
+        <v>0</v>
+      </c>
+      <c r="B24">
         <v>2010</v>
       </c>
-      <c r="C16" s="2">
+      <c r="C24">
         <v>1156312000</v>
       </c>
     </row>
-    <row r="17" spans="1:3">
-      <c r="A17" t="s">
-        <v>0</v>
-      </c>
-      <c r="B17">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A25" t="s">
+        <v>0</v>
+      </c>
+      <c r="B25">
         <v>2011</v>
       </c>
-      <c r="C17" s="2">
+      <c r="C25">
         <v>1161840000</v>
       </c>
     </row>
-    <row r="18" spans="1:3">
-      <c r="A18" t="s">
-        <v>0</v>
-      </c>
-      <c r="B18">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A26" t="s">
+        <v>0</v>
+      </c>
+      <c r="B26">
         <v>2012</v>
       </c>
-      <c r="C18" s="2"/>
-    </row>
-    <row r="19" spans="1:3">
-      <c r="A19" t="s">
-        <v>0</v>
-      </c>
-      <c r="B19">
+      <c r="C26">
+        <v>1153082000</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A27" t="s">
+        <v>0</v>
+      </c>
+      <c r="B27">
         <v>2013</v>
       </c>
-      <c r="C19" s="2">
+      <c r="C27">
         <v>1255182000</v>
       </c>
     </row>
-    <row r="20" spans="1:3">
-      <c r="A20" t="s">
-        <v>0</v>
-      </c>
-      <c r="B20">
+    <row r="28" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A28" t="s">
+        <v>0</v>
+      </c>
+      <c r="B28">
         <v>2014</v>
       </c>
-      <c r="C20" s="2">
+      <c r="C28">
         <v>1323472000</v>
       </c>
     </row>
-    <row r="21" spans="1:3">
-      <c r="A21" t="s">
-        <v>0</v>
-      </c>
-      <c r="B21">
+    <row r="29" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A29" t="s">
+        <v>0</v>
+      </c>
+      <c r="B29">
         <v>2015</v>
       </c>
-      <c r="C21" s="2">
+      <c r="C29">
         <v>1270769000</v>
       </c>
     </row>
-    <row r="22" spans="1:3">
-      <c r="A22" t="s">
-        <v>0</v>
-      </c>
-      <c r="B22">
+    <row r="30" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A30" t="s">
+        <v>0</v>
+      </c>
+      <c r="B30">
         <v>2016</v>
       </c>
-      <c r="C22" s="2">
+      <c r="C30">
         <v>1239757000</v>
       </c>
     </row>
-    <row r="23" spans="1:3">
-      <c r="A23" t="s">
-        <v>0</v>
-      </c>
-      <c r="B23">
+    <row r="31" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A31" t="s">
+        <v>0</v>
+      </c>
+      <c r="B31">
         <v>2017</v>
       </c>
-      <c r="C23" s="2">
+      <c r="C31">
         <v>1342765000</v>
       </c>
     </row>
-    <row r="24" spans="1:3">
-      <c r="A24" t="s">
-        <v>0</v>
-      </c>
-      <c r="B24">
+    <row r="32" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A32" t="s">
+        <v>0</v>
+      </c>
+      <c r="B32">
         <v>2018</v>
       </c>
-      <c r="C24" s="2">
+      <c r="C32">
         <v>1353368000</v>
       </c>
     </row>
-    <row r="25" spans="1:3">
-      <c r="A25" t="s">
-        <v>0</v>
-      </c>
-      <c r="B25">
+    <row r="33" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A33" t="s">
+        <v>0</v>
+      </c>
+      <c r="B33">
         <v>2019</v>
       </c>
-      <c r="C25" s="3">
+      <c r="C33">
         <v>1362825000</v>
       </c>
     </row>
-    <row r="26" spans="1:3">
-      <c r="A26" t="s">
-        <v>0</v>
-      </c>
-      <c r="B26">
+    <row r="34" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A34" t="s">
+        <v>0</v>
+      </c>
+      <c r="B34">
         <v>2020</v>
       </c>
-      <c r="C26" s="3">
+      <c r="C34">
         <v>1388392000</v>
       </c>
     </row>
-    <row r="27" spans="1:3">
-      <c r="A27" t="s">
-        <v>0</v>
-      </c>
-      <c r="B27">
+    <row r="35" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A35" t="s">
+        <v>0</v>
+      </c>
+      <c r="B35">
         <v>2021</v>
       </c>
-      <c r="C27" s="4">
+      <c r="C35">
         <v>1450341000</v>
       </c>
     </row>
-    <row r="28" spans="1:3">
-      <c r="A28" t="s">
-        <v>0</v>
-      </c>
-      <c r="B28">
+    <row r="36" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A36" t="s">
+        <v>0</v>
+      </c>
+      <c r="B36">
         <v>2022</v>
       </c>
-      <c r="C28" s="3">
+      <c r="C36">
         <v>2065254000</v>
       </c>
     </row>
-    <row r="29" spans="1:3">
-      <c r="A29" t="s">
-        <v>0</v>
-      </c>
-      <c r="B29">
+    <row r="37" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A37" t="s">
+        <v>0</v>
+      </c>
+      <c r="B37">
         <v>2023</v>
       </c>
-      <c r="C29" s="3">
+      <c r="C37">
         <v>1748368000</v>
       </c>
     </row>
   </sheetData>
+  <autoFilter ref="A1:C37" xr:uid="{09B6FE2E-2FCD-6348-B33B-60CC5A0315DF}">
+    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:C37">
+      <sortCondition ref="A1:A37"/>
+    </sortState>
+  </autoFilter>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>